<commit_message>
New shared general fcts
</commit_message>
<xml_diff>
--- a/00_additional_data/COS_chambers_sensor_logbook.xlsx
+++ b/00_additional_data/COS_chambers_sensor_logbook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="chambers" sheetId="4" r:id="rId1"/>
@@ -674,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -901,22 +901,22 @@
         <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fixed bad chamber removal
</commit_message>
<xml_diff>
--- a/00_additional_data/COS_chambers_sensor_logbook.xlsx
+++ b/00_additional_data/COS_chambers_sensor_logbook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="chambers" sheetId="4" r:id="rId1"/>
@@ -37,25 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
-  <si>
-    <t>b_irr1</t>
-  </si>
-  <si>
-    <t>b_con2</t>
-  </si>
-  <si>
-    <t>s_irr3</t>
-  </si>
-  <si>
-    <t>s_con4</t>
-  </si>
-  <si>
-    <t>s_irr5</t>
-  </si>
-  <si>
-    <t>s_con6</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>4 is irrigation</t>
   </si>
@@ -487,48 +469,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -557,7 +539,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="4"/>
       <c r="L2" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -585,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -598,10 +580,18 @@
       <c r="C4" s="2">
         <v>12</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
       <c r="H4" s="4">
         <v>0</v>
       </c>
@@ -612,7 +602,7 @@
         <v>0.72083333333333333</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -675,7 +665,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -686,28 +676,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -733,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -759,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -771,7 +761,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="6" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -781,7 +771,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -809,25 +799,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -850,7 +840,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -860,7 +850,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -887,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -898,28 +888,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -945,19 +935,33 @@
         <v>0</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="A3" s="1">
+        <v>44573</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Renamed con to ctr & added concentration symbol
</commit_message>
<xml_diff>
--- a/00_additional_data/COS_chambers_sensor_logbook.xlsx
+++ b/00_additional_data/COS_chambers_sensor_logbook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="chambers" sheetId="4" r:id="rId1"/>
@@ -37,13 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
-  <si>
-    <t>4 is irrigation</t>
-  </si>
-  <si>
-    <t>16 is control</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>comment</t>
   </si>
@@ -63,12 +57,6 @@
     <t>leaf.chb_irr1</t>
   </si>
   <si>
-    <t>leaf.chb_con2</t>
-  </si>
-  <si>
-    <t>air.chb_con2</t>
-  </si>
-  <si>
     <t>laserbox</t>
   </si>
   <si>
@@ -99,19 +87,25 @@
     <t>chb_irr1</t>
   </si>
   <si>
-    <t>chb_con2</t>
-  </si>
-  <si>
     <t>chs_irr3</t>
   </si>
   <si>
-    <t>chs_con4</t>
-  </si>
-  <si>
     <t>chs_irr5</t>
   </si>
   <si>
-    <t>chs_con6</t>
+    <t>chb_ctr2</t>
+  </si>
+  <si>
+    <t>chs_ctr4</t>
+  </si>
+  <si>
+    <t>chs_ctr6</t>
+  </si>
+  <si>
+    <t>leaf.chb_ctr2</t>
+  </si>
+  <si>
+    <t>air.chb_ctr2</t>
   </si>
 </sst>
 </file>
@@ -469,48 +463,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="L1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -539,7 +533,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="4"/>
       <c r="L2" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -567,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -602,7 +596,7 @@
         <v>0.72083333333333333</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -665,7 +659,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -676,28 +670,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -723,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -749,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -760,9 +754,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="6" t="s">
-        <v>0</v>
-      </c>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1"/>
@@ -770,9 +762,7 @@
       <c r="C5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="6" t="s">
-        <v>1</v>
-      </c>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1"/>
@@ -787,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="G1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -799,25 +789,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -840,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -850,7 +840,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -878,7 +868,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -888,28 +878,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -935,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -961,7 +951,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">

</xml_diff>